<commit_message>
Updated BOM and BOM list in Assembly Guide
</commit_message>
<xml_diff>
--- a/Documentation/Cedar_Mini_Joystick_BOM_v0.9.xlsx
+++ b/Documentation/Cedar_Mini_Joystick_BOM_v0.9.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-RD/Shared Documents/RD 23-05 ATP Joysticks/1B - Joystick - Mini/GitHub v0.9/Cedar_Mini_Joystick/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-RD/Shared Documents/RD 23-05 ATP Joysticks/1B - Joystick - Mini/Cedar_Mini_Joystick/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{E254BBE7-73FC-405C-B312-C48C0E4A8CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61CDDCF3-666F-440D-A75A-EFC0DA16F8B3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D88DF98C-70F1-4281-85E3-3681A9AD519E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="86">
+  <si>
+    <t>Cedar Mini Joystick</t>
+  </si>
   <si>
     <t>Unit Cost</t>
   </si>
@@ -52,6 +55,26 @@
     <t>Total filament (g)</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">Version: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>V1.0</t>
+    </r>
+  </si>
+  <si>
+    <t>Last Updated: 2023-June-30</t>
+  </si>
+  <si>
     <t>Commercial Parts</t>
   </si>
   <si>
@@ -88,10 +111,106 @@
     <t>Link</t>
   </si>
   <si>
+    <t>Joystick (PS2)</t>
+  </si>
+  <si>
+    <t>Electrical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.ca/dp/B089VXPHDH?_encoding=UTF8&amp;psc=1&amp;ref_=cm_sw_r_cp_ud_dp_GGTEDME4PM2P27SG86P7 </t>
+  </si>
+  <si>
+    <t>USB-C cable, 6 ft (can buy this locally)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/cvilux-usa/DH-20M50053/13177348 </t>
+  </si>
+  <si>
+    <t>Adafruit QT Py SAMD21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/adafruit-industries-llc/4600/13543375 </t>
+  </si>
+  <si>
+    <t>3.5 mm mono jack, panel mount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/cui-devices/MJ-3502/281321 </t>
+  </si>
+  <si>
+    <t>Slide switch, right angle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/c-k/OS102011MA1QS1/1981431 </t>
+  </si>
+  <si>
+    <t>Right angle female header, 5 position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/sullins-connector-solutions/PPTC051LGBN-RC/775899 </t>
+  </si>
+  <si>
+    <t>Female header, 7 position, single row, 0.100"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/sullins-connector-solutions/PPTC071LFBN-RC/810146 </t>
+  </si>
+  <si>
+    <t>#4 Metal Screw, 3/8″ Length (if building more than one, link below)</t>
+  </si>
+  <si>
     <t>Mechanical</t>
   </si>
   <si>
-    <t>Electrical</t>
+    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/serpac/6005/307599 </t>
+  </si>
+  <si>
+    <t>Wire, solid core, 1 foot, colour 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/cnc-tech/1007-24-1-2000-002-1-TD/17799208 </t>
+  </si>
+  <si>
+    <t>Wire, solid core, 1 foot, colour 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/cnc-tech/1007-24-1-2000-001-1-TD/17799235 </t>
+  </si>
+  <si>
+    <t>Wire, solid core, 1 foot, colour 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/cnc-tech/1007-24-1-2000-007-1-TD/17799170 </t>
+  </si>
+  <si>
+    <t>Ziptie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/te-connectivity/2-604771-9/2259327 </t>
+  </si>
+  <si>
+    <t>M3 hex nut x2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/keystone-electronics/4708/4499301 </t>
+  </si>
+  <si>
+    <t>(Optional for mount) M3x12mm screw x2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/apm-hexseal/RM3X12MM-2701/2063201 </t>
+  </si>
+  <si>
+    <t>(Optional for mount) Tee nut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.homedepot.ca/product/paulin-1-4-inch-20-tee-nuts-4-prong-5-16-inch-barrel-length/1000129429 </t>
+  </si>
+  <si>
+    <t>Digikey shipping (if spending less than $100)</t>
+  </si>
+  <si>
+    <t>Shipping</t>
   </si>
   <si>
     <t>3D Printed Parts                           ESTIMATED PRICING USING 1KG ROLL COST:</t>
@@ -115,9 +234,21 @@
     <t>Estimated Price</t>
   </si>
   <si>
+    <t>Enclosure bottom</t>
+  </si>
+  <si>
     <t>PLA</t>
   </si>
   <si>
+    <t>Enclosure top</t>
+  </si>
+  <si>
+    <t>3D PCB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slide switch </t>
+  </si>
+  <si>
     <t>Custom Printed Circuit Board (PCB)</t>
   </si>
   <si>
@@ -130,64 +261,43 @@
     <t>Part and description</t>
   </si>
   <si>
-    <t>Cedar Mini Joystick</t>
-  </si>
-  <si>
-    <t>Slide switch, right angle</t>
-  </si>
-  <si>
-    <t>Right angle female header, 5 position</t>
-  </si>
-  <si>
-    <t>3.5 mm mono jack, panel mount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/cui-devices/MJ-3502/281321 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/c-k/OS102011MA1QS1/1981431 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/sullins-connector-solutions/PPTC051LGBN-RC/775899 </t>
-  </si>
-  <si>
-    <t>Female header, 7 position, single row, 0.100"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/sullins-connector-solutions/PPTC071LFBN-RC/810146 </t>
-  </si>
-  <si>
     <t>#4 Metal Screw, 3/8″ Length, 100 pack</t>
   </si>
   <si>
     <t xml:space="preserve">https://a.co/d/523bJeL </t>
   </si>
   <si>
-    <t>Enclosure bottom</t>
-  </si>
-  <si>
-    <t>Enclosure top</t>
-  </si>
-  <si>
-    <t>3D PCB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slide switch </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/cnc-tech/3122-24-1-0500-007-1-TS/16396741 </t>
-  </si>
-  <si>
-    <t>Wire, 1 foot, colour 1</t>
-  </si>
-  <si>
-    <t>Wire, 1 foot, colour 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/cnc-tech/1569-26-1-0500-003-1-TS/15853701 </t>
-  </si>
-  <si>
-    <t>#4 Metal Screw, 3/8″ Length (if building more than one, link below)</t>
+    <t>USB-C cable, 3 feet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://a.co/d/97Y71JT </t>
+  </si>
+  <si>
+    <t>USB-C cable, 6 feet, 2 pack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://a.co/d/6UE2og9 </t>
+  </si>
+  <si>
+    <t>USB-C cable, 6 feet, 5 pack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://a.co/d/b3qG7jC </t>
+  </si>
+  <si>
+    <t>Zip tie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/heyco-products-corporation/13123B/15791902 </t>
+  </si>
+  <si>
+    <t>Number of joysticks:</t>
+  </si>
+  <si>
+    <t>Cost of materials for 2</t>
+  </si>
+  <si>
+    <t>Total Cost Each</t>
   </si>
   <si>
     <r>
@@ -207,103 +317,19 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/serpac/6005/307599 </t>
-  </si>
-  <si>
     <t>Last Updated: 2023-June-22</t>
   </si>
   <si>
-    <t>USB-C cable, 3 feet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://a.co/d/97Y71JT </t>
-  </si>
-  <si>
-    <t>USB-C cable, 6 feet, 5 pack</t>
-  </si>
-  <si>
-    <t>USB-C cable, 6 ft (can buy this locally)</t>
-  </si>
-  <si>
-    <t>USB-C cable, 6 feet, 2 pack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.ca/dp/B089VXPHDH?_encoding=UTF8&amp;psc=1&amp;ref_=cm_sw_r_cp_ud_dp_GGTEDME4PM2P27SG86P7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://a.co/d/6UE2og9 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://a.co/d/b3qG7jC </t>
-  </si>
-  <si>
-    <t>Number of joysticks:</t>
-  </si>
-  <si>
     <t>QTY per</t>
   </si>
   <si>
-    <t>Cost of materials for 2</t>
-  </si>
-  <si>
-    <t>Total Cost Each</t>
-  </si>
-  <si>
-    <t>Adafruit QT Py SAMD21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/adafruit-industries-llc/4600/13543375 </t>
-  </si>
-  <si>
-    <t>Ziptie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/te-connectivity/2-604771-9/2259327 </t>
-  </si>
-  <si>
-    <t>Zip tie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/heyco-products-corporation/13123B/15791902 </t>
-  </si>
-  <si>
-    <t>Joystick (PS2)</t>
-  </si>
-  <si>
-    <t>(Optional for mount) M3x12mm screw x2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/apm-hexseal/RM3X12MM-2701/2063201 </t>
-  </si>
-  <si>
-    <t>(Optional for mount) Tee nut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.homedepot.ca/product/paulin-1-4-inch-20-tee-nuts-4-prong-5-16-inch-barrel-length/1000129429 </t>
-  </si>
-  <si>
-    <t>Digikey shipping (if spending less than $100)</t>
-  </si>
-  <si>
-    <t>Shipping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/cvilux-usa/DH-20M50053/13177348 </t>
-  </si>
-  <si>
-    <t>M3 hex nut x2</t>
-  </si>
-  <si>
-    <t>Last Updated: 2023-June-30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.ca/en/products/detail/keystone-electronics/4708/4499301 </t>
+    <t>Cost of materials for 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -692,7 +718,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{7B4C5C8E-2942-4706-8013-CB2E3B3D0507}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -967,10 +995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N45"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,94 +1020,94 @@
   <sheetData>
     <row r="1" spans="1:13" ht="35.25" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="I2" s="25">
-        <f>SUM(I5:I20,I23:I28)</f>
-        <v>42.736500000000007</v>
+        <f>SUM(I5:I21,I24:I29)</f>
+        <v>42.726500000000001</v>
       </c>
       <c r="J2" s="5">
-        <f>SUM(J5:J21,I23:I28)</f>
-        <v>64.327500000000001</v>
+        <f>SUM(J5:J22,I24:I29)</f>
+        <v>64.317499999999995</v>
       </c>
       <c r="K2" s="16">
-        <f>SUM(H23:H27)/60</f>
+        <f>SUM(H24:H28)/60</f>
         <v>4.8833333333333337</v>
       </c>
       <c r="L2" s="6">
-        <f>SUM(E23:E27)</f>
+        <f>SUM(E24:E28)</f>
         <v>40.700000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="52" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" s="53"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1107,15 +1135,15 @@
         <v>23.99</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1143,15 +1171,15 @@
         <v>3.18</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1163,7 +1191,7 @@
         <v>10.79</v>
       </c>
       <c r="G7" s="46">
-        <f t="shared" ref="G7:G20" si="0">IF(E7&gt;0,ROUNDUP(D7/E7,0),0)</f>
+        <f t="shared" ref="G7:G21" si="0">IF(E7&gt;0,ROUNDUP(D7/E7,0),0)</f>
         <v>1</v>
       </c>
       <c r="H7" s="24">
@@ -1175,19 +1203,19 @@
         <v>10.79</v>
       </c>
       <c r="J7" s="23">
-        <f t="shared" ref="J7:J20" si="3">G7*F7</f>
+        <f t="shared" ref="J7:J21" si="3">G7*F7</f>
         <v>10.79</v>
       </c>
       <c r="K7" s="47" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -1215,15 +1243,15 @@
         <v>6.9599999999999991</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1251,15 +1279,15 @@
         <v>0.75</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1287,15 +1315,15 @@
         <v>0.93</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -1323,15 +1351,15 @@
         <v>1.7</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D12">
         <v>8</v>
@@ -1359,15 +1387,15 @@
         <v>4.8</v>
       </c>
       <c r="K12" s="47" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1376,34 +1404,34 @@
         <v>1</v>
       </c>
       <c r="F13" s="33">
-        <v>0.7</v>
+        <v>0.47</v>
       </c>
       <c r="G13" s="22">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H13" s="14">
-        <f t="shared" ref="H13:H20" si="4">IF(E13&gt;0,F13/E13,0)</f>
-        <v>0.7</v>
+        <f t="shared" ref="H13:H21" si="4">IF(E13&gt;0,F13/E13,0)</f>
+        <v>0.47</v>
       </c>
       <c r="I13" s="14">
-        <f t="shared" ref="I13:I20" si="5">H13*D13</f>
-        <v>0.7</v>
+        <f t="shared" ref="I13:I21" si="5">H13*D13</f>
+        <v>0.47</v>
       </c>
       <c r="J13" s="23">
         <f t="shared" si="3"/>
-        <v>0.7</v>
+        <v>0.47</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1412,7 +1440,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="33">
-        <v>0.72</v>
+        <v>0.47</v>
       </c>
       <c r="G14" s="22">
         <f t="shared" si="0"/>
@@ -1420,26 +1448,26 @@
       </c>
       <c r="H14" s="14">
         <f t="shared" si="4"/>
-        <v>0.72</v>
+        <v>0.47</v>
       </c>
       <c r="I14" s="14">
         <f t="shared" si="5"/>
-        <v>0.72</v>
+        <v>0.47</v>
       </c>
       <c r="J14" s="23">
         <f t="shared" si="3"/>
-        <v>0.72</v>
+        <v>0.47</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1448,122 +1476,122 @@
         <v>1</v>
       </c>
       <c r="F15" s="33">
-        <v>0.25</v>
+        <v>0.47</v>
       </c>
       <c r="G15" s="22">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H15" s="14">
         <f t="shared" si="4"/>
-        <v>0.25</v>
+        <v>0.47</v>
       </c>
       <c r="I15" s="14">
         <f t="shared" si="5"/>
-        <v>0.25</v>
+        <v>0.47</v>
       </c>
       <c r="J15" s="23">
         <f t="shared" si="3"/>
-        <v>0.25</v>
+        <v>0.47</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16" s="33">
-        <v>0.27</v>
-      </c>
-      <c r="G16" s="49">
-        <f t="shared" ref="G16:G19" si="6">IF(E16&gt;0,ROUNDUP(D16/E16,0),0)</f>
-        <v>2</v>
+        <v>0.25</v>
+      </c>
+      <c r="G16" s="22">
+        <v>1</v>
       </c>
       <c r="H16" s="14">
         <f t="shared" si="4"/>
-        <v>0.27</v>
+        <v>0.25</v>
       </c>
       <c r="I16" s="14">
         <f t="shared" si="5"/>
-        <v>0.54</v>
+        <v>0.25</v>
       </c>
       <c r="J16" s="23">
         <f t="shared" si="3"/>
-        <v>0.54</v>
+        <v>0.25</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="33">
+        <v>0.27</v>
+      </c>
+      <c r="G17" s="49">
+        <f t="shared" ref="G17:G20" si="6">IF(E17&gt;0,ROUNDUP(D17/E17,0),0)</f>
+        <v>2</v>
+      </c>
+      <c r="H17" s="14">
+        <f t="shared" si="4"/>
+        <v>0.27</v>
+      </c>
+      <c r="I17" s="14">
+        <f t="shared" si="5"/>
+        <v>0.54</v>
+      </c>
+      <c r="J17" s="23">
+        <f t="shared" si="3"/>
+        <v>0.54</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18">
         <v>0</v>
       </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17" s="33">
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" s="33">
         <v>1.1100000000000001</v>
       </c>
-      <c r="G17" s="49">
+      <c r="G18" s="49">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H17" s="14">
+      <c r="H18" s="14">
         <f t="shared" si="4"/>
         <v>1.1100000000000001</v>
-      </c>
-      <c r="I17" s="14">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="23">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18" s="51">
-        <v>0.48</v>
-      </c>
-      <c r="G18" s="22">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="14">
-        <f t="shared" si="4"/>
-        <v>0.48</v>
       </c>
       <c r="I18" s="14">
         <f t="shared" si="5"/>
@@ -1574,541 +1602,578 @@
         <v>0</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19" s="51">
-        <v>8</v>
+        <v>0.48</v>
       </c>
       <c r="G19" s="22">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" s="14">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>0.48</v>
       </c>
       <c r="I19" s="14">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J19" s="23">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" s="51">
         <v>8</v>
       </c>
-      <c r="K19" s="8"/>
-    </row>
-    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="18"/>
       <c r="G20" s="22">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="H20" s="14">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="I20" s="14">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="J20" s="23">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="K20" s="8"/>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="18"/>
+      <c r="G21" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H21" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I20" s="14">
+      <c r="I21" s="14">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J20" s="23">
+      <c r="J21" s="23">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="54" t="s">
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="55"/>
+      <c r="C22" s="26">
+        <v>25</v>
+      </c>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="N22" s="8"/>
+    </row>
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="K23" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="B21" s="55"/>
-      <c r="C21" s="26">
-        <v>25</v>
-      </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="N21" s="8"/>
-    </row>
-    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I22" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K22" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>20.2</v>
-      </c>
-      <c r="F23">
-        <v>149</v>
-      </c>
-      <c r="H23">
-        <f>F23*D23</f>
-        <v>149</v>
-      </c>
-      <c r="I23" s="14">
-        <f>(D23*E23/1000)*$C$21</f>
-        <v>0.505</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
-      <c r="E24" s="34">
-        <v>11.9</v>
+      <c r="E24">
+        <v>20.2</v>
       </c>
       <c r="F24">
-        <v>79</v>
+        <v>149</v>
       </c>
       <c r="H24">
-        <f t="shared" ref="H24:H26" si="7">F24*D24</f>
-        <v>79</v>
+        <f>F24*D24</f>
+        <v>149</v>
       </c>
       <c r="I24" s="14">
-        <f t="shared" ref="I24:I28" si="8">(D24*E24/1000)*$C$21</f>
-        <v>0.29750000000000004</v>
+        <f>(D24*E24/1000)*$C$22</f>
+        <v>0.505</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" s="34">
+        <v>11.9</v>
+      </c>
+      <c r="F25">
+        <v>79</v>
+      </c>
+      <c r="H25">
+        <f t="shared" ref="H25:H27" si="7">F25*D25</f>
+        <v>79</v>
+      </c>
+      <c r="I25" s="14">
+        <f t="shared" ref="I25:I29" si="8">(D25*E25/1000)*$C$22</f>
+        <v>0.29750000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="34">
         <v>8</v>
       </c>
-      <c r="F25">
+      <c r="F26">
         <v>57</v>
       </c>
-      <c r="H25">
+      <c r="H26">
         <f t="shared" si="7"/>
         <v>57</v>
       </c>
-      <c r="I25" s="14">
+      <c r="I26" s="14">
         <f t="shared" si="8"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
         <v>0.6</v>
       </c>
-      <c r="F26">
+      <c r="F27">
         <v>8</v>
       </c>
-      <c r="H26">
+      <c r="H27">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="I26" s="14">
+      <c r="I27" s="14">
         <f t="shared" si="8"/>
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I27" s="14">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="11"/>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I28" s="14">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="56" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="57"/>
-      <c r="I29" s="21"/>
+      <c r="B29" s="11"/>
+      <c r="I29" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29" t="s">
+      <c r="A30" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="57"/>
+      <c r="I30" s="21"/>
+    </row>
+    <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="31"/>
-    </row>
-    <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="11"/>
-      <c r="I31" s="21"/>
+      <c r="B31" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="31"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="54" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" s="55"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
-    </row>
-    <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="58" t="s">
-        <v>28</v>
-      </c>
-      <c r="B39" s="59"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
-    </row>
+      <c r="B32" s="11"/>
+      <c r="I32" s="21"/>
+    </row>
+    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="55"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+    </row>
+    <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B40" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="7" t="s">
+      <c r="A40" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="59"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
+    </row>
+    <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E40" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="7" t="s">
+      <c r="B41" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G40" s="7" t="s">
+      <c r="D41" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H40" s="7" t="s">
+      <c r="E41" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I40" s="7" t="s">
+      <c r="F41" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J40" s="7" t="s">
+      <c r="G41" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="K40" s="19" t="s">
+      <c r="H41" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>39</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="I41" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J41" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D41">
-        <v>8</v>
-      </c>
-      <c r="E41">
-        <v>100</v>
-      </c>
-      <c r="F41" s="33">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="G41" s="22">
-        <f>IF(E41&gt;0,ROUNDUP(D41/E41,0),0)</f>
-        <v>1</v>
-      </c>
-      <c r="H41" s="24">
-        <f>IF(E41&gt;0,F41/E41,0)</f>
-        <v>9.3000000000000013E-2</v>
-      </c>
-      <c r="I41" s="24">
-        <f>H41*D41</f>
-        <v>0.74400000000000011</v>
-      </c>
-      <c r="J41" s="23">
-        <f>G41*F41</f>
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="K41" s="8" t="s">
-        <v>40</v>
+      <c r="K41" s="19" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="C42" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F42" s="33">
-        <v>9.5</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="G42" s="22">
-        <f t="shared" ref="G42:G45" si="9">IF(E42&gt;0,ROUNDUP(D42/E42,0),0)</f>
+        <f>IF(E42&gt;0,ROUNDUP(D42/E42,0),0)</f>
         <v>1</v>
       </c>
       <c r="H42" s="24">
         <f>IF(E42&gt;0,F42/E42,0)</f>
-        <v>9.5</v>
+        <v>9.3000000000000013E-2</v>
       </c>
       <c r="I42" s="24">
         <f>H42*D42</f>
-        <v>9.5</v>
+        <v>0.74400000000000011</v>
       </c>
       <c r="J42" s="23">
         <f>G42*F42</f>
-        <v>9.5</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C43" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
       <c r="E43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" s="33">
-        <v>12.99</v>
+        <v>9.5</v>
       </c>
       <c r="G43" s="22">
-        <f t="shared" ref="G43" si="10">IF(E43&gt;0,ROUNDUP(D43/E43,0),0)</f>
+        <f t="shared" ref="G43:G46" si="9">IF(E43&gt;0,ROUNDUP(D43/E43,0),0)</f>
         <v>1</v>
       </c>
       <c r="H43" s="24">
         <f>IF(E43&gt;0,F43/E43,0)</f>
-        <v>6.4950000000000001</v>
+        <v>9.5</v>
       </c>
       <c r="I43" s="24">
         <f>H43*D43</f>
-        <v>6.4950000000000001</v>
+        <v>9.5</v>
       </c>
       <c r="J43" s="23">
         <f>G43*F43</f>
-        <v>12.99</v>
+        <v>9.5</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="C44" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F44" s="33">
-        <v>19.989999999999998</v>
+        <v>12.99</v>
       </c>
       <c r="G44" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="G44" si="10">IF(E44&gt;0,ROUNDUP(D44/E44,0),0)</f>
         <v>1</v>
       </c>
       <c r="H44" s="24">
         <f>IF(E44&gt;0,F44/E44,0)</f>
-        <v>3.9979999999999998</v>
+        <v>6.4950000000000001</v>
       </c>
       <c r="I44" s="24">
         <f>H44*D44</f>
-        <v>3.9979999999999998</v>
+        <v>6.4950000000000001</v>
       </c>
       <c r="J44" s="23">
         <f>G44*F44</f>
-        <v>19.989999999999998</v>
+        <v>12.99</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C45" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D45">
         <v>1</v>
       </c>
       <c r="E45">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F45" s="33">
-        <v>0.15</v>
-      </c>
-      <c r="G45" s="49">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="G45" s="22">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="H45" s="50">
+      <c r="H45" s="24">
         <f>IF(E45&gt;0,F45/E45,0)</f>
-        <v>0.15</v>
-      </c>
-      <c r="I45" s="50">
+        <v>3.9979999999999998</v>
+      </c>
+      <c r="I45" s="24">
         <f>H45*D45</f>
-        <v>0.15</v>
+        <v>3.9979999999999998</v>
       </c>
       <c r="J45" s="23">
         <f>G45*F45</f>
+        <v>19.989999999999998</v>
+      </c>
+      <c r="K45" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46" s="33">
         <v>0.15</v>
       </c>
-      <c r="K45" s="8" t="s">
-        <v>70</v>
+      <c r="G46" s="49">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="H46" s="50">
+        <f>IF(E46&gt;0,F46/E46,0)</f>
+        <v>0.15</v>
+      </c>
+      <c r="I46" s="50">
+        <f>H46*D46</f>
+        <v>0.15</v>
+      </c>
+      <c r="J46" s="23">
+        <f>G46*F46</f>
+        <v>0.15</v>
+      </c>
+      <c r="K46" s="8" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A40:B40"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K8" r:id="rId1" xr:uid="{E3DEF1DD-6029-4056-B3FB-98F7C207AE92}"/>
     <hyperlink ref="K9" r:id="rId2" xr:uid="{0F3D00AF-9352-4DAE-BB11-3DEED1DEE812}"/>
     <hyperlink ref="K10" r:id="rId3" xr:uid="{E168B8A8-09F8-4BC7-BE4A-BAB88B85CE77}"/>
     <hyperlink ref="K11" r:id="rId4" xr:uid="{AB8B4906-0100-475A-A810-6553B6BAE213}"/>
-    <hyperlink ref="K41" r:id="rId5" xr:uid="{28C384D9-3092-4894-99A6-3A08F0266E61}"/>
-    <hyperlink ref="K13" r:id="rId6" xr:uid="{3DF9DD6F-6633-40A4-9BD7-4BF77974D58C}"/>
-    <hyperlink ref="K14" r:id="rId7" xr:uid="{38308223-4A9E-459D-9944-DEF5BE3680A4}"/>
-    <hyperlink ref="K12" r:id="rId8" xr:uid="{24F7BAAE-E59B-4ED5-A1CD-50F90C951085}"/>
-    <hyperlink ref="K42" r:id="rId9" xr:uid="{34965F44-DF18-4E43-80C4-2AADE880F8C3}"/>
-    <hyperlink ref="K5" r:id="rId10" xr:uid="{149EAE72-EE50-40F8-8D53-3054C66B3F0A}"/>
-    <hyperlink ref="K43" r:id="rId11" xr:uid="{4A847862-4FA8-4495-834C-EA245D2D4277}"/>
-    <hyperlink ref="K44" r:id="rId12" xr:uid="{A2F8BAFA-5753-4446-8CF2-9D687763C1DA}"/>
-    <hyperlink ref="K7" r:id="rId13" xr:uid="{3FAEE428-9FB1-46C9-91A7-274E1BB75FA5}"/>
-    <hyperlink ref="K15" r:id="rId14" xr:uid="{14CF58C7-290C-4B13-ABF3-8C043918B96D}"/>
-    <hyperlink ref="K45" r:id="rId15" xr:uid="{3A99E3B6-C86E-49FB-A5B2-A920C0568C23}"/>
-    <hyperlink ref="K18" r:id="rId16" xr:uid="{742A2295-AAD6-42F4-B819-8BDFE53DA400}"/>
-    <hyperlink ref="K17" r:id="rId17" xr:uid="{077D6F57-CE43-4517-9725-BAC63E5846CB}"/>
-    <hyperlink ref="K6" r:id="rId18" xr:uid="{E1E74B8C-B5B9-4715-9878-46584B5F0BB3}"/>
-    <hyperlink ref="K16" r:id="rId19" xr:uid="{14CC92AF-C0C8-4296-9E58-10FFCC20ABF4}"/>
+    <hyperlink ref="K42" r:id="rId5" xr:uid="{28C384D9-3092-4894-99A6-3A08F0266E61}"/>
+    <hyperlink ref="K12" r:id="rId6" xr:uid="{24F7BAAE-E59B-4ED5-A1CD-50F90C951085}"/>
+    <hyperlink ref="K43" r:id="rId7" xr:uid="{34965F44-DF18-4E43-80C4-2AADE880F8C3}"/>
+    <hyperlink ref="K5" r:id="rId8" xr:uid="{149EAE72-EE50-40F8-8D53-3054C66B3F0A}"/>
+    <hyperlink ref="K44" r:id="rId9" xr:uid="{4A847862-4FA8-4495-834C-EA245D2D4277}"/>
+    <hyperlink ref="K45" r:id="rId10" xr:uid="{A2F8BAFA-5753-4446-8CF2-9D687763C1DA}"/>
+    <hyperlink ref="K7" r:id="rId11" xr:uid="{3FAEE428-9FB1-46C9-91A7-274E1BB75FA5}"/>
+    <hyperlink ref="K16" r:id="rId12" xr:uid="{14CF58C7-290C-4B13-ABF3-8C043918B96D}"/>
+    <hyperlink ref="K46" r:id="rId13" xr:uid="{3A99E3B6-C86E-49FB-A5B2-A920C0568C23}"/>
+    <hyperlink ref="K19" r:id="rId14" xr:uid="{742A2295-AAD6-42F4-B819-8BDFE53DA400}"/>
+    <hyperlink ref="K18" r:id="rId15" xr:uid="{077D6F57-CE43-4517-9725-BAC63E5846CB}"/>
+    <hyperlink ref="K6" r:id="rId16" xr:uid="{E1E74B8C-B5B9-4715-9878-46584B5F0BB3}"/>
+    <hyperlink ref="K17" r:id="rId17" xr:uid="{A683A31C-5A07-4296-B3B5-61CA84E9A955}"/>
+    <hyperlink ref="K13" r:id="rId18" xr:uid="{82E0F021-032A-4B35-9E7E-DB90A8F8D55B}"/>
+    <hyperlink ref="K14" r:id="rId19" xr:uid="{65E31250-7E08-4889-87A8-F4B5720910BE}"/>
+    <hyperlink ref="K15" r:id="rId20" xr:uid="{5C5801FB-471C-460C-B7A9-B26190E3FD86}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A5ED6DE-856F-4FDE-898B-9C661E55648B}">
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="B13" sqref="B13:L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2131,123 +2196,123 @@
   <sheetData>
     <row r="1" spans="1:14" ht="35.25" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="I1" s="43" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="K1" s="36" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L1" s="44" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="M1" s="37" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N1" s="38" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="E2">
         <v>2</v>
       </c>
       <c r="I2" s="39">
         <f>J2/E2</f>
-        <v>34.672999999999995</v>
+        <v>34.66299999999999</v>
       </c>
       <c r="J2" s="39">
-        <f>SUM(J5:J20,J23:J28)</f>
-        <v>69.345999999999989</v>
+        <f>SUM(J5:J21,J24:J29)</f>
+        <v>69.325999999999979</v>
       </c>
       <c r="K2" s="40">
-        <f>SUM(K5:K21,J23:J28)</f>
-        <v>96.35</v>
+        <f>SUM(K5:K22,J24:J29)</f>
+        <v>96.329999999999984</v>
       </c>
       <c r="L2" s="45">
         <f>K2/E2</f>
-        <v>48.174999999999997</v>
+        <v>48.164999999999992</v>
       </c>
       <c r="M2" s="41">
-        <f>SUM(I23:I27)/60</f>
+        <f>SUM(I24:I28)/60</f>
         <v>9.6999999999999993</v>
       </c>
       <c r="N2" s="42">
-        <f>SUM(F23:F27)</f>
+        <f>SUM(F24:F28)</f>
         <v>40.400000000000006</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="52" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" s="53"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E19" si="0">D5*$E$2</f>
+        <f t="shared" ref="E5:E20" si="0">D5*$E$2</f>
         <v>2</v>
       </c>
       <c r="F5">
@@ -2273,15 +2338,15 @@
         <v>23.99</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -2297,31 +2362,31 @@
         <v>3.18</v>
       </c>
       <c r="H6" s="22">
-        <f t="shared" ref="H6:H19" si="1">IF(F6&gt;0,ROUNDUP(E6/F6,0),0)</f>
+        <f t="shared" ref="H6:H20" si="1">IF(F6&gt;0,ROUNDUP(E6/F6,0),0)</f>
         <v>2</v>
       </c>
       <c r="I6" s="24">
-        <f t="shared" ref="I6:I19" si="2">IF(F6&gt;0,G6/F6,0)</f>
+        <f t="shared" ref="I6:I20" si="2">IF(F6&gt;0,G6/F6,0)</f>
         <v>3.18</v>
       </c>
       <c r="J6" s="24">
-        <f t="shared" ref="J6:J19" si="3">I6*E6</f>
+        <f t="shared" ref="J6:J20" si="3">I6*E6</f>
         <v>6.36</v>
       </c>
       <c r="K6" s="23">
-        <f t="shared" ref="K6:K19" si="4">H6*G6</f>
+        <f t="shared" ref="K6:K20" si="4">H6*G6</f>
         <v>6.36</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -2353,15 +2418,15 @@
         <v>21.58</v>
       </c>
       <c r="L7" s="47" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -2393,15 +2458,15 @@
         <v>13.919999999999998</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -2433,15 +2498,15 @@
         <v>1.5</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -2473,15 +2538,15 @@
         <v>1.86</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -2513,15 +2578,15 @@
         <v>3.4</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D12">
         <v>8</v>
@@ -2553,15 +2618,15 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="L12" s="47" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -2574,7 +2639,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="33">
-        <v>0.7</v>
+        <v>0.47</v>
       </c>
       <c r="H13" s="22">
         <f t="shared" si="1"/>
@@ -2582,26 +2647,26 @@
       </c>
       <c r="I13" s="24">
         <f t="shared" si="2"/>
-        <v>0.7</v>
+        <v>0.47</v>
       </c>
       <c r="J13" s="24">
         <f t="shared" si="3"/>
-        <v>1.4</v>
+        <v>0.94</v>
       </c>
       <c r="K13" s="23">
         <f t="shared" si="4"/>
-        <v>1.4</v>
+        <v>0.94</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -2614,7 +2679,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="33">
-        <v>0.72</v>
+        <v>0.47</v>
       </c>
       <c r="H14" s="22">
         <f t="shared" si="1"/>
@@ -2622,26 +2687,26 @@
       </c>
       <c r="I14" s="24">
         <f t="shared" si="2"/>
-        <v>0.72</v>
+        <v>0.47</v>
       </c>
       <c r="J14" s="24">
         <f t="shared" si="3"/>
-        <v>1.44</v>
+        <v>0.94</v>
       </c>
       <c r="K14" s="23">
         <f t="shared" si="4"/>
-        <v>1.44</v>
+        <v>0.94</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -2654,7 +2719,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="33">
-        <v>0.25</v>
+        <v>0.47</v>
       </c>
       <c r="H15" s="22">
         <f t="shared" si="1"/>
@@ -2662,106 +2727,106 @@
       </c>
       <c r="I15" s="24">
         <f t="shared" si="2"/>
-        <v>0.25</v>
+        <v>0.47</v>
       </c>
       <c r="J15" s="24">
         <f t="shared" si="3"/>
-        <v>0.5</v>
+        <v>0.94</v>
       </c>
       <c r="K15" s="23">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0.94</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16" s="33">
-        <v>0.27</v>
+        <v>0.25</v>
       </c>
       <c r="H16" s="22">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I16" s="24">
         <f t="shared" si="2"/>
-        <v>0.27</v>
+        <v>0.25</v>
       </c>
       <c r="J16" s="24">
         <f t="shared" si="3"/>
-        <v>1.08</v>
+        <v>0.5</v>
       </c>
       <c r="K16" s="23">
         <f t="shared" si="4"/>
-        <v>1.08</v>
+        <v>0.5</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17" s="33">
-        <v>1.1100000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="H17" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I17" s="24">
         <f t="shared" si="2"/>
-        <v>1.1100000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="J17" s="24">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.08</v>
       </c>
       <c r="K17" s="23">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.08</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2773,8 +2838,8 @@
       <c r="F18">
         <v>1</v>
       </c>
-      <c r="G18" s="51">
-        <v>0.48</v>
+      <c r="G18" s="33">
+        <v>1.1100000000000001</v>
       </c>
       <c r="H18" s="22">
         <f t="shared" si="1"/>
@@ -2782,7 +2847,7 @@
       </c>
       <c r="I18" s="24">
         <f t="shared" si="2"/>
-        <v>0.48</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="J18" s="24">
         <f t="shared" si="3"/>
@@ -2793,194 +2858,205 @@
         <v>0</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" s="51">
+        <v>0.48</v>
+      </c>
+      <c r="H19" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="24">
+        <f t="shared" si="2"/>
+        <v>0.48</v>
+      </c>
+      <c r="J19" s="24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="23">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20">
         <f>1/$E$2</f>
         <v>0.5</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19" s="51">
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" s="51">
         <v>8</v>
       </c>
-      <c r="H19" s="22">
+      <c r="H20" s="22">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I19" s="24">
+      <c r="I20" s="24">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="J19" s="24">
+      <c r="J20" s="24">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="K19" s="23">
+      <c r="K20" s="23">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="L19" s="8"/>
-    </row>
-    <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G20" s="33"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="23"/>
       <c r="L20" s="8"/>
     </row>
     <row r="21" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="54" t="s">
+      <c r="G21" s="33"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="8"/>
+    </row>
+    <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="55"/>
+      <c r="C22" s="26">
+        <v>25</v>
+      </c>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="O22" s="8"/>
+    </row>
+    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="J23" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="L23" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="B21" s="55"/>
-      <c r="C21" s="26">
-        <v>25</v>
-      </c>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="O21" s="8"/>
-    </row>
-    <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J22" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L22" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <f>D23*$E$2</f>
-        <v>2</v>
-      </c>
-      <c r="F23">
-        <v>20.2</v>
-      </c>
-      <c r="G23">
-        <v>150</v>
-      </c>
-      <c r="I23">
-        <f>G23*E23</f>
-        <v>300</v>
-      </c>
-      <c r="J23" s="14">
-        <f>(E23*F23/1000)*$C$21</f>
-        <v>1.01</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24">
-        <f t="shared" ref="E24:E26" si="5">D24*$E$2</f>
+        <f>D24*$E$2</f>
         <v>2</v>
       </c>
-      <c r="F24" s="34">
-        <v>12</v>
+      <c r="F24">
+        <v>20.2</v>
       </c>
       <c r="G24">
-        <v>79</v>
+        <v>150</v>
       </c>
       <c r="I24">
-        <f t="shared" ref="I24:I26" si="6">G24*E24</f>
-        <v>158</v>
+        <f>G24*E24</f>
+        <v>300</v>
       </c>
       <c r="J24" s="14">
-        <f t="shared" ref="J24:J26" si="7">(E24*F24/1000)*$C$21</f>
-        <v>0.6</v>
+        <f>(E24*F24/1000)*$C$22</f>
+        <v>1.01</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="E25:E27" si="5">D25*$E$2</f>
         <v>2</v>
       </c>
-      <c r="F25">
-        <v>7.6</v>
+      <c r="F25" s="34">
+        <v>12</v>
       </c>
       <c r="G25">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="I25">
-        <f t="shared" si="6"/>
-        <v>108</v>
+        <f t="shared" ref="I25:I27" si="6">G25*E25</f>
+        <v>158</v>
       </c>
       <c r="J25" s="14">
-        <f t="shared" si="7"/>
-        <v>0.38</v>
+        <f t="shared" ref="J25:J27" si="7">(E25*F25/1000)*$C$22</f>
+        <v>0.6</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -2990,262 +3066,255 @@
         <v>2</v>
       </c>
       <c r="F26">
-        <v>0.6</v>
+        <v>7.6</v>
       </c>
       <c r="G26">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="I26">
         <f t="shared" si="6"/>
-        <v>16</v>
+        <v>108</v>
       </c>
       <c r="J26" s="14">
         <f t="shared" si="7"/>
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>0.6</v>
+      </c>
+      <c r="G27">
+        <v>8</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="J27" s="14">
+        <f t="shared" si="7"/>
         <v>0.03</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J27" s="14">
-        <f t="shared" ref="J27:J28" si="8">(D27*F27/1000)*$C$21</f>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J28" s="14">
+        <f t="shared" ref="J28:J29" si="8">(D28*F28/1000)*$C$22</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="11"/>
-      <c r="J28" s="14">
+    <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="11"/>
+      <c r="J29" s="14">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="56" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="57"/>
-      <c r="J29" s="21"/>
-    </row>
     <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29" t="s">
+      <c r="A30" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="57"/>
+      <c r="J30" s="21"/>
+    </row>
+    <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="31"/>
-    </row>
-    <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="11"/>
-      <c r="J31" s="21"/>
+      <c r="B31" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="31"/>
     </row>
     <row r="32" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="54" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" s="55"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
-      <c r="O32" s="10"/>
-    </row>
-    <row r="38" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="58" t="s">
-        <v>28</v>
-      </c>
-      <c r="B39" s="59"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
-    </row>
+      <c r="B32" s="11"/>
+      <c r="J32" s="21"/>
+    </row>
+    <row r="33" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="55"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+    </row>
+    <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B40" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="7" t="s">
+      <c r="A40" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="59"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="10"/>
+    </row>
+    <row r="41" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G40" s="7" t="s">
+      <c r="B41" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H40" s="7" t="s">
+      <c r="D41" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I40" s="7" t="s">
+      <c r="E41" s="7"/>
+      <c r="F41" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J40" s="7" t="s">
+      <c r="G41" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="K40" s="7" t="s">
+      <c r="H41" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L40" s="19" t="s">
+      <c r="I41" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>39</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="J41" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K41" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D41">
-        <v>8</v>
-      </c>
-      <c r="F41">
-        <v>100</v>
-      </c>
-      <c r="G41" s="33">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="H41" s="22">
-        <f>IF(F41&gt;0,ROUNDUP(D41/F41,0),0)</f>
-        <v>1</v>
-      </c>
-      <c r="I41" s="24">
-        <f>IF(F41&gt;0,G41/F41,0)</f>
-        <v>9.3000000000000013E-2</v>
-      </c>
-      <c r="J41" s="24">
-        <f>I41*D41</f>
-        <v>0.74400000000000011</v>
-      </c>
-      <c r="K41" s="23">
-        <f>H41*G41</f>
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="L41" s="8" t="s">
-        <v>40</v>
+      <c r="L41" s="19" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="C42" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G42" s="33">
-        <v>9.5</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="H42" s="22">
-        <f t="shared" ref="H42:H44" si="9">IF(F42&gt;0,ROUNDUP(D42/F42,0),0)</f>
+        <f>IF(F42&gt;0,ROUNDUP(D42/F42,0),0)</f>
         <v>1</v>
       </c>
       <c r="I42" s="24">
         <f>IF(F42&gt;0,G42/F42,0)</f>
-        <v>9.5</v>
+        <v>9.3000000000000013E-2</v>
       </c>
       <c r="J42" s="24">
         <f>I42*D42</f>
-        <v>9.5</v>
+        <v>0.74400000000000011</v>
       </c>
       <c r="K42" s="23">
         <f>H42*G42</f>
-        <v>9.5</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C43" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
       <c r="F43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G43" s="33">
-        <v>12.99</v>
+        <v>9.5</v>
       </c>
       <c r="H43" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="H43:H45" si="9">IF(F43&gt;0,ROUNDUP(D43/F43,0),0)</f>
         <v>1</v>
       </c>
       <c r="I43" s="24">
         <f>IF(F43&gt;0,G43/F43,0)</f>
-        <v>6.4950000000000001</v>
+        <v>9.5</v>
       </c>
       <c r="J43" s="24">
         <f>I43*D43</f>
-        <v>6.4950000000000001</v>
+        <v>9.5</v>
       </c>
       <c r="K43" s="23">
         <f>H43*G43</f>
-        <v>12.99</v>
+        <v>9.5</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="C44" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="F44">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G44" s="33">
-        <v>19.989999999999998</v>
+        <v>12.99</v>
       </c>
       <c r="H44" s="22">
         <f t="shared" si="9"/>
@@ -3253,59 +3322,96 @@
       </c>
       <c r="I44" s="24">
         <f>IF(F44&gt;0,G44/F44,0)</f>
-        <v>3.9979999999999998</v>
+        <v>6.4950000000000001</v>
       </c>
       <c r="J44" s="24">
         <f>I44*D44</f>
-        <v>3.9979999999999998</v>
+        <v>6.4950000000000001</v>
       </c>
       <c r="K44" s="23">
         <f>H44*G44</f>
+        <v>12.99</v>
+      </c>
+      <c r="L44" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>5</v>
+      </c>
+      <c r="G45" s="33">
         <v>19.989999999999998</v>
       </c>
-      <c r="L44" s="8" t="s">
-        <v>60</v>
+      <c r="H45" s="22">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="I45" s="24">
+        <f>IF(F45&gt;0,G45/F45,0)</f>
+        <v>3.9979999999999998</v>
+      </c>
+      <c r="J45" s="24">
+        <f>I45*D45</f>
+        <v>3.9979999999999998</v>
+      </c>
+      <c r="K45" s="23">
+        <f>H45*G45</f>
+        <v>19.989999999999998</v>
+      </c>
+      <c r="L45" s="8" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A40:B40"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L8" r:id="rId1" xr:uid="{724508D6-18E0-4095-B47F-BFF30F769829}"/>
     <hyperlink ref="L9" r:id="rId2" xr:uid="{9473194B-E6A0-4990-94D7-0C220030D18C}"/>
     <hyperlink ref="L10" r:id="rId3" xr:uid="{FDBDB31C-B422-4E9A-AA65-ED1E97DAEB82}"/>
     <hyperlink ref="L11" r:id="rId4" xr:uid="{E2974EE9-98D5-41AE-AA99-2E90B7D25F4F}"/>
-    <hyperlink ref="L41" r:id="rId5" xr:uid="{1E24F24C-ADB4-4AE2-A05B-FD61E79D998D}"/>
-    <hyperlink ref="L13" r:id="rId6" xr:uid="{E0EAE085-37A2-40F4-B8A0-BCF1E3706419}"/>
-    <hyperlink ref="L14" r:id="rId7" xr:uid="{AEE6ECCA-E4BD-4512-AEEB-652E74650615}"/>
-    <hyperlink ref="L42" r:id="rId8" xr:uid="{1D0B8ED3-0DCC-4782-9041-17D4D95191EC}"/>
-    <hyperlink ref="L5" r:id="rId9" xr:uid="{00CFDCA8-1667-4EB0-AE0E-7E72C2D96F94}"/>
-    <hyperlink ref="L43" r:id="rId10" xr:uid="{BB5BB40D-BA2C-4386-9428-F04D037C94BE}"/>
-    <hyperlink ref="L44" r:id="rId11" xr:uid="{EA20526D-1547-4F0B-81A7-C4D5CE52A2AF}"/>
-    <hyperlink ref="L12" r:id="rId12" xr:uid="{B30873B4-62C0-4021-9338-A2DFBC9861B5}"/>
-    <hyperlink ref="L7" r:id="rId13" xr:uid="{022E48E9-F149-41DF-A04D-CE9ACB4A074E}"/>
-    <hyperlink ref="L15" r:id="rId14" xr:uid="{EFA7CC8D-FB10-4CD0-8DC5-B8A377E3B80C}"/>
-    <hyperlink ref="L18" r:id="rId15" xr:uid="{22E9464D-5956-4F03-A226-0C003F892E4F}"/>
-    <hyperlink ref="L17" r:id="rId16" xr:uid="{400DADB6-677F-4AEA-B0A6-AA20AF41EF34}"/>
-    <hyperlink ref="L6" r:id="rId17" xr:uid="{E84C4678-65AB-4871-B605-63FF3D6E9CD6}"/>
-    <hyperlink ref="L16" r:id="rId18" xr:uid="{89A450DD-36F6-440F-8464-21B6FE678318}"/>
+    <hyperlink ref="L42" r:id="rId5" xr:uid="{1E24F24C-ADB4-4AE2-A05B-FD61E79D998D}"/>
+    <hyperlink ref="L43" r:id="rId6" xr:uid="{1D0B8ED3-0DCC-4782-9041-17D4D95191EC}"/>
+    <hyperlink ref="L5" r:id="rId7" xr:uid="{00CFDCA8-1667-4EB0-AE0E-7E72C2D96F94}"/>
+    <hyperlink ref="L44" r:id="rId8" xr:uid="{BB5BB40D-BA2C-4386-9428-F04D037C94BE}"/>
+    <hyperlink ref="L45" r:id="rId9" xr:uid="{EA20526D-1547-4F0B-81A7-C4D5CE52A2AF}"/>
+    <hyperlink ref="L12" r:id="rId10" xr:uid="{B30873B4-62C0-4021-9338-A2DFBC9861B5}"/>
+    <hyperlink ref="L7" r:id="rId11" xr:uid="{022E48E9-F149-41DF-A04D-CE9ACB4A074E}"/>
+    <hyperlink ref="L16" r:id="rId12" xr:uid="{EFA7CC8D-FB10-4CD0-8DC5-B8A377E3B80C}"/>
+    <hyperlink ref="L19" r:id="rId13" xr:uid="{22E9464D-5956-4F03-A226-0C003F892E4F}"/>
+    <hyperlink ref="L18" r:id="rId14" xr:uid="{400DADB6-677F-4AEA-B0A6-AA20AF41EF34}"/>
+    <hyperlink ref="L6" r:id="rId15" xr:uid="{E84C4678-65AB-4871-B605-63FF3D6E9CD6}"/>
+    <hyperlink ref="L17" r:id="rId16" xr:uid="{DCE02CF0-0B07-4D32-ADDA-AB481A67C4AE}"/>
+    <hyperlink ref="L13" r:id="rId17" xr:uid="{B0BD1328-EE57-4D39-ACEB-4A61C38E3016}"/>
+    <hyperlink ref="L14" r:id="rId18" xr:uid="{A25B8BFF-CB49-4F1A-9942-26136E327DC3}"/>
+    <hyperlink ref="L15" r:id="rId19" xr:uid="{4C7013DE-ECA5-4ECE-8ECD-70A80E69AD86}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D858965-35F5-4E4C-9CAB-B979BF5BD61C}">
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3328,117 +3434,117 @@
   <sheetData>
     <row r="1" spans="1:14" ht="35.25" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="I1" s="43" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="K1" s="36" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L1" s="44" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="M1" s="37" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N1" s="38" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="E2">
         <v>5</v>
       </c>
       <c r="I2" s="39">
         <f>J2/E2</f>
-        <v>30.672999999999995</v>
+        <v>30.662999999999993</v>
       </c>
       <c r="J2" s="39">
-        <f>SUM(J5:J20,J23:J28)</f>
-        <v>153.36499999999998</v>
+        <f>SUM(J5:J21,J24:J29)</f>
+        <v>153.31499999999997</v>
       </c>
       <c r="K2" s="40">
-        <f>SUM(K5:K21,J23:J28)</f>
-        <v>170.93999999999997</v>
+        <f>SUM(K5:K22,J24:J29)</f>
+        <v>170.88999999999996</v>
       </c>
       <c r="L2" s="45">
         <f>K2/E2</f>
-        <v>34.187999999999995</v>
+        <v>34.17799999999999</v>
       </c>
       <c r="M2" s="41">
-        <f>SUM(I23:I27)/60</f>
+        <f>SUM(I24:I28)/60</f>
         <v>24.25</v>
       </c>
       <c r="N2" s="42">
-        <f>SUM(F23:F27)</f>
+        <f>SUM(F24:F28)</f>
         <v>40.400000000000006</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="52" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" s="53"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -3470,15 +3576,15 @@
         <v>23.99</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -3510,15 +3616,15 @@
         <v>15.9</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -3534,37 +3640,37 @@
         <v>10.79</v>
       </c>
       <c r="H7" s="22">
-        <f t="shared" ref="H7:H19" si="5">IF(F7&gt;0,ROUNDUP(E7/F7,0),0)</f>
+        <f t="shared" ref="H7:H20" si="5">IF(F7&gt;0,ROUNDUP(E7/F7,0),0)</f>
         <v>5</v>
       </c>
       <c r="I7" s="24">
-        <f t="shared" ref="I7:I19" si="6">IF(F7&gt;0,G7/F7,0)</f>
+        <f t="shared" ref="I7:I20" si="6">IF(F7&gt;0,G7/F7,0)</f>
         <v>10.79</v>
       </c>
       <c r="J7" s="24">
-        <f t="shared" ref="J7:J19" si="7">I7*E7</f>
+        <f t="shared" ref="J7:J20" si="7">I7*E7</f>
         <v>53.949999999999996</v>
       </c>
       <c r="K7" s="23">
-        <f t="shared" ref="K7:K19" si="8">H7*G7</f>
+        <f t="shared" ref="K7:K20" si="8">H7*G7</f>
         <v>53.949999999999996</v>
       </c>
       <c r="L7" s="47" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>3</v>
       </c>
       <c r="E8">
-        <f t="shared" ref="E8:E19" si="9">D8*$E$2</f>
+        <f t="shared" ref="E8:E20" si="9">D8*$E$2</f>
         <v>15</v>
       </c>
       <c r="F8">
@@ -3590,15 +3696,15 @@
         <v>34.799999999999997</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -3630,15 +3736,15 @@
         <v>3.75</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -3670,15 +3776,15 @@
         <v>4.6500000000000004</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -3710,15 +3816,15 @@
         <v>8.5</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D12">
         <v>8</v>
@@ -3750,15 +3856,15 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="L12" s="47" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -3771,7 +3877,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="33">
-        <v>0.7</v>
+        <v>0.47</v>
       </c>
       <c r="H13" s="22">
         <f t="shared" si="5"/>
@@ -3779,26 +3885,26 @@
       </c>
       <c r="I13" s="24">
         <f t="shared" si="6"/>
-        <v>0.7</v>
+        <v>0.47</v>
       </c>
       <c r="J13" s="24">
         <f t="shared" si="7"/>
-        <v>3.5</v>
+        <v>2.3499999999999996</v>
       </c>
       <c r="K13" s="23">
         <f t="shared" si="8"/>
-        <v>3.5</v>
+        <v>2.3499999999999996</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -3811,7 +3917,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="33">
-        <v>0.72</v>
+        <v>0.47</v>
       </c>
       <c r="H14" s="22">
         <f t="shared" si="5"/>
@@ -3819,26 +3925,26 @@
       </c>
       <c r="I14" s="24">
         <f t="shared" si="6"/>
-        <v>0.72</v>
+        <v>0.47</v>
       </c>
       <c r="J14" s="24">
         <f t="shared" si="7"/>
-        <v>3.5999999999999996</v>
+        <v>2.3499999999999996</v>
       </c>
       <c r="K14" s="23">
         <f t="shared" si="8"/>
-        <v>3.5999999999999996</v>
+        <v>2.3499999999999996</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -3851,7 +3957,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="33">
-        <v>0.25</v>
+        <v>0.47</v>
       </c>
       <c r="H15" s="22">
         <f t="shared" si="5"/>
@@ -3859,106 +3965,106 @@
       </c>
       <c r="I15" s="24">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0.47</v>
       </c>
       <c r="J15" s="24">
         <f t="shared" si="7"/>
-        <v>1.25</v>
+        <v>2.3499999999999996</v>
       </c>
       <c r="K15" s="23">
         <f t="shared" si="8"/>
-        <v>1.25</v>
+        <v>2.3499999999999996</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <f t="shared" si="9"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16" s="33">
-        <v>0.27</v>
+        <v>0.25</v>
       </c>
       <c r="H16" s="22">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I16" s="24">
         <f t="shared" si="6"/>
-        <v>0.27</v>
+        <v>0.25</v>
       </c>
       <c r="J16" s="24">
         <f t="shared" si="7"/>
-        <v>2.7</v>
+        <v>1.25</v>
       </c>
       <c r="K16" s="23">
         <f t="shared" si="8"/>
-        <v>2.7</v>
+        <v>1.25</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E17">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17" s="33">
-        <v>1.1100000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="H17" s="22">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I17" s="24">
         <f t="shared" si="6"/>
-        <v>1.1100000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="J17" s="24">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="K17" s="23">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -3970,8 +4076,8 @@
       <c r="F18">
         <v>1</v>
       </c>
-      <c r="G18" s="51">
-        <v>0.48</v>
+      <c r="G18" s="33">
+        <v>1.1100000000000001</v>
       </c>
       <c r="H18" s="22">
         <f t="shared" si="5"/>
@@ -3979,7 +4085,7 @@
       </c>
       <c r="I18" s="24">
         <f t="shared" si="6"/>
-        <v>0.48</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="J18" s="24">
         <f t="shared" si="7"/>
@@ -3990,15 +4096,15 @@
         <v>0</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -4011,7 +4117,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="51">
-        <v>8</v>
+        <v>0.48</v>
       </c>
       <c r="H19" s="22">
         <f t="shared" si="5"/>
@@ -4019,7 +4125,7 @@
       </c>
       <c r="I19" s="24">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>0.48</v>
       </c>
       <c r="J19" s="24">
         <f t="shared" si="7"/>
@@ -4029,155 +4135,165 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="L19" s="8"/>
-    </row>
-    <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G20" s="33"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="23"/>
+      <c r="L19" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" s="51">
+        <v>8</v>
+      </c>
+      <c r="H20" s="22">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="24">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="J20" s="24">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="23">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="L20" s="8"/>
     </row>
     <row r="21" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="54" t="s">
+      <c r="G21" s="33"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="8"/>
+    </row>
+    <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="55"/>
+      <c r="C22" s="26">
+        <v>25</v>
+      </c>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="O22" s="8"/>
+    </row>
+    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="J23" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="L23" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="B21" s="55"/>
-      <c r="C21" s="26">
-        <v>25</v>
-      </c>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="O21" s="8"/>
-    </row>
-    <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J22" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L22" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <f>D23*$E$2</f>
-        <v>5</v>
-      </c>
-      <c r="F23">
-        <v>20.2</v>
-      </c>
-      <c r="G23">
-        <v>150</v>
-      </c>
-      <c r="I23">
-        <f>G23*E23</f>
-        <v>750</v>
-      </c>
-      <c r="J23" s="14">
-        <f>(E23*F23/1000)*$C$21</f>
-        <v>2.5250000000000004</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24">
-        <f t="shared" ref="E24:E26" si="10">D24*$E$2</f>
+        <f>D24*$E$2</f>
         <v>5</v>
       </c>
-      <c r="F24" s="34">
-        <v>12</v>
+      <c r="F24">
+        <v>20.2</v>
       </c>
       <c r="G24">
-        <v>79</v>
+        <v>150</v>
       </c>
       <c r="I24">
-        <f t="shared" ref="I24:I26" si="11">G24*E24</f>
-        <v>395</v>
+        <f>G24*E24</f>
+        <v>750</v>
       </c>
       <c r="J24" s="14">
-        <f t="shared" ref="J24:J26" si="12">(E24*F24/1000)*$C$21</f>
-        <v>1.5</v>
+        <f>(E24*F24/1000)*$C$22</f>
+        <v>2.5250000000000004</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="E25:E27" si="10">D25*$E$2</f>
         <v>5</v>
       </c>
-      <c r="F25">
-        <v>7.6</v>
+      <c r="F25" s="34">
+        <v>12</v>
       </c>
       <c r="G25">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="I25">
-        <f t="shared" si="11"/>
-        <v>270</v>
+        <f t="shared" ref="I25:I27" si="11">G25*E25</f>
+        <v>395</v>
       </c>
       <c r="J25" s="14">
-        <f t="shared" si="12"/>
-        <v>0.95</v>
-      </c>
-      <c r="M25" s="23"/>
+        <f t="shared" ref="J25:J27" si="12">(E25*F25/1000)*$C$22</f>
+        <v>1.5</v>
+      </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -4187,263 +4303,257 @@
         <v>5</v>
       </c>
       <c r="F26">
-        <v>0.6</v>
+        <v>7.6</v>
       </c>
       <c r="G26">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="I26">
         <f t="shared" si="11"/>
-        <v>40</v>
+        <v>270</v>
       </c>
       <c r="J26" s="14">
         <f t="shared" si="12"/>
+        <v>0.95</v>
+      </c>
+      <c r="M26" s="23"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="F27">
+        <v>0.6</v>
+      </c>
+      <c r="G27">
+        <v>8</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="11"/>
+        <v>40</v>
+      </c>
+      <c r="J27" s="14">
+        <f t="shared" si="12"/>
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J27" s="14">
-        <f t="shared" ref="J27:J28" si="13">(D27*F27/1000)*$C$21</f>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J28" s="14">
+        <f t="shared" ref="J28:J29" si="13">(D28*F28/1000)*$C$22</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="11"/>
-      <c r="D28" s="23"/>
-      <c r="J28" s="14">
+    <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="11"/>
+      <c r="D29" s="23"/>
+      <c r="J29" s="14">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="56" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="57"/>
-      <c r="J29" s="21"/>
-    </row>
     <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29" t="s">
+      <c r="A30" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="57"/>
+      <c r="J30" s="21"/>
+    </row>
+    <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="31"/>
-    </row>
-    <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="11"/>
-      <c r="J31" s="21"/>
+      <c r="B31" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="31"/>
     </row>
     <row r="32" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="54" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" s="55"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
-      <c r="O32" s="10"/>
-    </row>
-    <row r="38" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="58" t="s">
-        <v>28</v>
-      </c>
-      <c r="B39" s="59"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
-    </row>
+      <c r="B32" s="11"/>
+      <c r="J32" s="21"/>
+    </row>
+    <row r="33" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="55"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+    </row>
+    <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B40" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="7" t="s">
+      <c r="A40" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="59"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="10"/>
+    </row>
+    <row r="41" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G40" s="7" t="s">
+      <c r="B41" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H40" s="7" t="s">
+      <c r="D41" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I40" s="7" t="s">
+      <c r="E41" s="7"/>
+      <c r="F41" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J40" s="7" t="s">
+      <c r="G41" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="K40" s="7" t="s">
+      <c r="H41" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L40" s="19" t="s">
+      <c r="I41" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>39</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="J41" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K41" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D41">
-        <v>8</v>
-      </c>
-      <c r="F41">
-        <v>100</v>
-      </c>
-      <c r="G41" s="33">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="H41" s="22">
-        <f>IF(F41&gt;0,ROUNDUP(D41/F41,0),0)</f>
-        <v>1</v>
-      </c>
-      <c r="I41" s="24">
-        <f>IF(F41&gt;0,G41/F41,0)</f>
-        <v>9.3000000000000013E-2</v>
-      </c>
-      <c r="J41" s="24">
-        <f>I41*D41</f>
-        <v>0.74400000000000011</v>
-      </c>
-      <c r="K41" s="23">
-        <f>H41*G41</f>
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="L41" s="8" t="s">
-        <v>40</v>
+      <c r="L41" s="19" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="C42" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G42" s="33">
-        <v>9.5</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="H42" s="22">
-        <f t="shared" ref="H42:H44" si="14">IF(F42&gt;0,ROUNDUP(D42/F42,0),0)</f>
+        <f>IF(F42&gt;0,ROUNDUP(D42/F42,0),0)</f>
         <v>1</v>
       </c>
       <c r="I42" s="24">
         <f>IF(F42&gt;0,G42/F42,0)</f>
-        <v>9.5</v>
+        <v>9.3000000000000013E-2</v>
       </c>
       <c r="J42" s="24">
         <f>I42*D42</f>
-        <v>9.5</v>
+        <v>0.74400000000000011</v>
       </c>
       <c r="K42" s="23">
         <f>H42*G42</f>
-        <v>9.5</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C43" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
       <c r="F43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G43" s="33">
-        <v>12.99</v>
+        <v>9.5</v>
       </c>
       <c r="H43" s="22">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="H43:H45" si="14">IF(F43&gt;0,ROUNDUP(D43/F43,0),0)</f>
         <v>1</v>
       </c>
       <c r="I43" s="24">
         <f>IF(F43&gt;0,G43/F43,0)</f>
-        <v>6.4950000000000001</v>
+        <v>9.5</v>
       </c>
       <c r="J43" s="24">
         <f>I43*D43</f>
-        <v>6.4950000000000001</v>
+        <v>9.5</v>
       </c>
       <c r="K43" s="23">
         <f>H43*G43</f>
-        <v>12.99</v>
+        <v>9.5</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="C44" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="F44">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G44" s="33">
-        <v>19.989999999999998</v>
+        <v>12.99</v>
       </c>
       <c r="H44" s="22">
         <f t="shared" si="14"/>
@@ -4451,54 +4561,102 @@
       </c>
       <c r="I44" s="24">
         <f>IF(F44&gt;0,G44/F44,0)</f>
-        <v>3.9979999999999998</v>
+        <v>6.4950000000000001</v>
       </c>
       <c r="J44" s="24">
         <f>I44*D44</f>
-        <v>3.9979999999999998</v>
+        <v>6.4950000000000001</v>
       </c>
       <c r="K44" s="23">
         <f>H44*G44</f>
+        <v>12.99</v>
+      </c>
+      <c r="L44" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>5</v>
+      </c>
+      <c r="G45" s="33">
         <v>19.989999999999998</v>
       </c>
-      <c r="L44" s="8" t="s">
-        <v>60</v>
+      <c r="H45" s="22">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="I45" s="24">
+        <f>IF(F45&gt;0,G45/F45,0)</f>
+        <v>3.9979999999999998</v>
+      </c>
+      <c r="J45" s="24">
+        <f>I45*D45</f>
+        <v>3.9979999999999998</v>
+      </c>
+      <c r="K45" s="23">
+        <f>H45*G45</f>
+        <v>19.989999999999998</v>
+      </c>
+      <c r="L45" s="8" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A40:B40"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L8" r:id="rId1" xr:uid="{AD73D34B-BD9A-4303-8819-34B5C3E166EF}"/>
     <hyperlink ref="L9" r:id="rId2" xr:uid="{5B548D2E-9258-4B4D-98EF-4382D3D5A547}"/>
     <hyperlink ref="L10" r:id="rId3" xr:uid="{088475F5-409B-4714-AABD-FA88A6808844}"/>
     <hyperlink ref="L11" r:id="rId4" xr:uid="{607B36CA-57FD-4253-A6AD-57E5B2378594}"/>
-    <hyperlink ref="L41" r:id="rId5" xr:uid="{69FF048B-979A-4C87-8EC1-6CA9554EC32B}"/>
-    <hyperlink ref="L13" r:id="rId6" xr:uid="{E5EA6EE4-BDF3-4B17-8959-CBB98414561C}"/>
-    <hyperlink ref="L14" r:id="rId7" xr:uid="{C21E7D1B-E239-4206-8898-7663806C72C6}"/>
-    <hyperlink ref="L42" r:id="rId8" xr:uid="{386D690F-2D09-4CDD-87D3-9917158478A4}"/>
-    <hyperlink ref="L5" r:id="rId9" xr:uid="{7C079CBC-1DA8-4662-BE18-7D943BACAFA2}"/>
-    <hyperlink ref="L43" r:id="rId10" xr:uid="{471BBC8E-C768-4555-8435-0195E83E9D14}"/>
-    <hyperlink ref="L44" r:id="rId11" xr:uid="{0DC93975-6CCE-4F7A-946A-817F7DA198C7}"/>
-    <hyperlink ref="L12" r:id="rId12" xr:uid="{84E0F963-1AC5-488E-983E-3BDE5E06B239}"/>
-    <hyperlink ref="L7" r:id="rId13" xr:uid="{93A9FA8F-492A-45CC-ABA4-3BC13ED25FCD}"/>
-    <hyperlink ref="L15" r:id="rId14" xr:uid="{C9CF054A-5B17-49DC-9E19-661F793364CA}"/>
-    <hyperlink ref="L18" r:id="rId15" xr:uid="{D08D93DC-E154-4A30-A24F-CC3D79D13268}"/>
-    <hyperlink ref="L17" r:id="rId16" xr:uid="{7EA83F58-F50F-4B36-BD61-64A8089ACFF1}"/>
-    <hyperlink ref="L6" r:id="rId17" xr:uid="{F8647EA7-0811-4F16-8C3C-371BBDD9D346}"/>
-    <hyperlink ref="L16" r:id="rId18" xr:uid="{9D11DD56-B9F5-4A47-8117-2DBCBDF82C22}"/>
+    <hyperlink ref="L42" r:id="rId5" xr:uid="{69FF048B-979A-4C87-8EC1-6CA9554EC32B}"/>
+    <hyperlink ref="L43" r:id="rId6" xr:uid="{386D690F-2D09-4CDD-87D3-9917158478A4}"/>
+    <hyperlink ref="L5" r:id="rId7" xr:uid="{7C079CBC-1DA8-4662-BE18-7D943BACAFA2}"/>
+    <hyperlink ref="L44" r:id="rId8" xr:uid="{471BBC8E-C768-4555-8435-0195E83E9D14}"/>
+    <hyperlink ref="L45" r:id="rId9" xr:uid="{0DC93975-6CCE-4F7A-946A-817F7DA198C7}"/>
+    <hyperlink ref="L12" r:id="rId10" xr:uid="{84E0F963-1AC5-488E-983E-3BDE5E06B239}"/>
+    <hyperlink ref="L7" r:id="rId11" xr:uid="{93A9FA8F-492A-45CC-ABA4-3BC13ED25FCD}"/>
+    <hyperlink ref="L16" r:id="rId12" xr:uid="{C9CF054A-5B17-49DC-9E19-661F793364CA}"/>
+    <hyperlink ref="L19" r:id="rId13" xr:uid="{D08D93DC-E154-4A30-A24F-CC3D79D13268}"/>
+    <hyperlink ref="L18" r:id="rId14" xr:uid="{7EA83F58-F50F-4B36-BD61-64A8089ACFF1}"/>
+    <hyperlink ref="L6" r:id="rId15" xr:uid="{F8647EA7-0811-4F16-8C3C-371BBDD9D346}"/>
+    <hyperlink ref="L17" r:id="rId16" xr:uid="{F6BB9DA2-09CE-4A11-ABE2-A173CEAFF41C}"/>
+    <hyperlink ref="L13" r:id="rId17" xr:uid="{583B50E7-071A-481E-BC78-EB7AD220B2A9}"/>
+    <hyperlink ref="L14" r:id="rId18" xr:uid="{8E22A132-C0D7-4EBF-9BDC-0F34D95A8729}"/>
+    <hyperlink ref="L15" r:id="rId19" xr:uid="{3F1B2F09-EEEF-4F1D-81B2-A83395F67C55}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B51EC7ECFAC78D4E8EF6CBAFFF0B3505" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7e0d9d996845e2cef65e12e895c4c91e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e" xmlns:ns3="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="97eb945ec045b4d52e9ff03a8a8db852" ns2:_="" ns3:_="">
     <xsd:import namespace="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
@@ -4741,7 +4899,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4750,18 +4908,18 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="72c39c84-b0a3-45a2-a38c-ff46bb47f11f"/>
+    <ds:schemaRef ds:uri="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C86E4E0D-DC31-4848-BC7A-F0ECE7F7EB00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4780,21 +4938,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="72c39c84-b0a3-45a2-a38c-ff46bb47f11f"/>
-    <ds:schemaRef ds:uri="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>